<commit_message>
STOP, interfaz y correo de saldo
</commit_message>
<xml_diff>
--- a/proyectomensajes/mensajes.xlsx
+++ b/proyectomensajes/mensajes.xlsx
@@ -397,55 +397,1166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>$__</v>
+        <v>COD_CLI</v>
       </c>
       <c r="B1" t="str">
-        <v>$isNew</v>
+        <v>APELLIDOS_NOMBRES</v>
       </c>
       <c r="C1" t="str">
-        <v>_doc</v>
+        <v>NRO_CEL</v>
+      </c>
+      <c r="D1" t="str">
+        <v>PLAZA</v>
+      </c>
+      <c r="E1" t="str">
+        <v>AGENCIA</v>
+      </c>
+      <c r="F1" t="str">
+        <v>MENSAJE</v>
+      </c>
+      <c r="G1" t="str">
+        <v>FECHA_ENVIO</v>
+      </c>
+      <c r="H1" t="str">
+        <v>HORA_ENVIO</v>
+      </c>
+      <c r="I1" t="str">
+        <v>ENVIADOR</v>
+      </c>
+      <c r="J1" t="str">
+        <v>CHIP</v>
       </c>
     </row>
     <row r="2">
-      <c r="B2" t="b">
-        <v>0</v>
+      <c r="A2">
+        <v>70218</v>
+      </c>
+      <c r="B2" t="str">
+        <v>ROMERO BOLIVAR MIRTHA ANDREA</v>
+      </c>
+      <c r="C2">
+        <v>72241497</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2" t="str">
+        <v>30</v>
+      </c>
+      <c r="F2" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G2" t="str">
+        <v>13/1/2023</v>
+      </c>
+      <c r="H2" t="str">
+        <v>11:17:43</v>
+      </c>
+      <c r="I2" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J2">
+        <v>73348513</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" t="b">
-        <v>0</v>
+      <c r="A3">
+        <v>70220</v>
+      </c>
+      <c r="B3" t="str">
+        <v>TERRAZAS MONTERO GUIDO RAUL</v>
+      </c>
+      <c r="C3">
+        <v>77439601</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3" t="str">
+        <v>30</v>
+      </c>
+      <c r="F3" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G3" t="str">
+        <v>13/1/2023</v>
+      </c>
+      <c r="H3" t="str">
+        <v>11:34:4</v>
+      </c>
+      <c r="I3" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J3">
+        <v>73348513</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" t="b">
-        <v>0</v>
+      <c r="A4">
+        <v>70220</v>
+      </c>
+      <c r="B4" t="str">
+        <v>TERRAZAS MONTERO GUIDO RAUL</v>
+      </c>
+      <c r="C4">
+        <v>77439601</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4" t="str">
+        <v>30</v>
+      </c>
+      <c r="F4" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G4" t="str">
+        <v>13/1/2023</v>
+      </c>
+      <c r="H4" t="str">
+        <v>11:40:9</v>
+      </c>
+      <c r="I4" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J4">
+        <v>73348513</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" t="b">
-        <v>0</v>
+      <c r="A5">
+        <v>70220</v>
+      </c>
+      <c r="B5" t="str">
+        <v>TERRAZAS MONTERO GUIDO RAUL</v>
+      </c>
+      <c r="C5">
+        <v>77439601</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5" t="str">
+        <v>30</v>
+      </c>
+      <c r="F5" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G5" t="str">
+        <v>13/1/2023</v>
+      </c>
+      <c r="H5" t="str">
+        <v>11:54:15</v>
+      </c>
+      <c r="I5" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J5">
+        <v>73348513</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" t="b">
-        <v>0</v>
+      <c r="A6">
+        <v>70218</v>
+      </c>
+      <c r="B6" t="str">
+        <v>ROMERO BOLIVAR MIRTHA ANDREA</v>
+      </c>
+      <c r="C6">
+        <v>72241497</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="E6" t="str">
+        <v>30</v>
+      </c>
+      <c r="F6" t="str">
+        <v>VPR-ASFI Te invita a participar en la Encuesta Nacional de Servicios Financieros 2022 del 1/Dic al 31/Dic haz clic en: https://encuesta2022.asfi.gob.bo</v>
+      </c>
+      <c r="G6" t="str">
+        <v>13/1/2023</v>
+      </c>
+      <c r="H6" t="str">
+        <v>13:12:50</v>
+      </c>
+      <c r="I6" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J6">
+        <v>73348513</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" t="b">
-        <v>0</v>
+      <c r="A7">
+        <v>70218</v>
+      </c>
+      <c r="B7" t="str">
+        <v>ROMERO BOLIVAR MIRTHA ANDREA</v>
+      </c>
+      <c r="C7">
+        <v>72241497</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="E7" t="str">
+        <v>30</v>
+      </c>
+      <c r="F7" t="str">
+        <v>creamos un mensaje</v>
+      </c>
+      <c r="G7" t="str">
+        <v>16/1/2023</v>
+      </c>
+      <c r="H7" t="str">
+        <v>22:24:50</v>
+      </c>
+      <c r="I7" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J7">
+        <v>73348513</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>70218</v>
+      </c>
+      <c r="B8" t="str">
+        <v>ROMERO BOLIVAR MIRTHA ANDREA</v>
+      </c>
+      <c r="C8">
+        <v>72241497</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="E8" t="str">
+        <v>30</v>
+      </c>
+      <c r="F8" t="str">
+        <v>VPR-ASFI Te invita a participar en la Encuesta Nacional de Servicios Financieros 2022 del 1/Dic al 31/Dic haz clic en: https://encuesta2022.asfi.gob.bo</v>
+      </c>
+      <c r="G8" t="str">
+        <v>17/1/2023</v>
+      </c>
+      <c r="H8" t="str">
+        <v>13:12:33</v>
+      </c>
+      <c r="I8" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J8">
+        <v>73348513</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>70218</v>
+      </c>
+      <c r="B9" t="str">
+        <v>ROMERO BOLIVAR MIRTHA ANDREA</v>
+      </c>
+      <c r="C9">
+        <v>72241497</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9" t="str">
+        <v>30</v>
+      </c>
+      <c r="F9" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G9" t="str">
+        <v>19/1/2023</v>
+      </c>
+      <c r="H9" t="str">
+        <v>17:17:43</v>
+      </c>
+      <c r="I9" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J9">
+        <v>73348513</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>20711</v>
+      </c>
+      <c r="B10" t="str">
+        <v>COSSIO DE DIAZ ROSSY FANNY</v>
+      </c>
+      <c r="C10">
+        <v>72206061</v>
+      </c>
+      <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="E10" t="str">
+        <v>20</v>
+      </c>
+      <c r="F10" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G10" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H10" t="str">
+        <v>9:33:56</v>
+      </c>
+      <c r="I10" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J10">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>21502</v>
+      </c>
+      <c r="B11" t="str">
+        <v>COSSIO REY FABRICIO CRISTOBAL</v>
+      </c>
+      <c r="C11">
+        <v>76796433</v>
+      </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+      <c r="E11" t="str">
+        <v>20</v>
+      </c>
+      <c r="F11" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G11" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H11" t="str">
+        <v>9:33:58</v>
+      </c>
+      <c r="I11" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J11">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>39001</v>
+      </c>
+      <c r="B12" t="str">
+        <v>TORRICO SILES DE TEJERINA NANCY ROSARIO</v>
+      </c>
+      <c r="C12">
+        <v>70346980</v>
+      </c>
+      <c r="D12">
+        <v>30</v>
+      </c>
+      <c r="E12" t="str">
+        <v>20</v>
+      </c>
+      <c r="F12" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G12" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H12" t="str">
+        <v>9:34:0</v>
+      </c>
+      <c r="I12" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J12">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>2892</v>
+      </c>
+      <c r="B13" t="str">
+        <v>VARGAS ANGULO WILMER FRANCISCO</v>
+      </c>
+      <c r="C13">
+        <v>72777758</v>
+      </c>
+      <c r="D13">
+        <v>30</v>
+      </c>
+      <c r="E13" t="str">
+        <v>20</v>
+      </c>
+      <c r="F13" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G13" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H13" t="str">
+        <v>9:34:2</v>
+      </c>
+      <c r="I13" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J13">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>20711</v>
+      </c>
+      <c r="B14" t="str">
+        <v>COSSIO DE DIAZ ROSSY FANNY</v>
+      </c>
+      <c r="C14">
+        <v>72206061</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
+      <c r="E14" t="str">
+        <v>20</v>
+      </c>
+      <c r="F14" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G14" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H14" t="str">
+        <v>9:34:4</v>
+      </c>
+      <c r="I14" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J14">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>21502</v>
+      </c>
+      <c r="B15" t="str">
+        <v>COSSIO REY FABRICIO CRISTOBAL</v>
+      </c>
+      <c r="C15">
+        <v>76796433</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+      <c r="E15" t="str">
+        <v>20</v>
+      </c>
+      <c r="F15" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G15" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H15" t="str">
+        <v>9:34:6</v>
+      </c>
+      <c r="I15" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J15">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>39001</v>
+      </c>
+      <c r="B16" t="str">
+        <v>TORRICO SILES DE TEJERINA NANCY ROSARIO</v>
+      </c>
+      <c r="C16">
+        <v>70346980</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+      <c r="E16" t="str">
+        <v>20</v>
+      </c>
+      <c r="F16" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G16" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H16" t="str">
+        <v>9:34:8</v>
+      </c>
+      <c r="I16" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J16">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>2892</v>
+      </c>
+      <c r="B17" t="str">
+        <v>VARGAS ANGULO WILMER FRANCISCO</v>
+      </c>
+      <c r="C17">
+        <v>72777758</v>
+      </c>
+      <c r="D17">
+        <v>30</v>
+      </c>
+      <c r="E17" t="str">
+        <v>20</v>
+      </c>
+      <c r="F17" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G17" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H17" t="str">
+        <v>9:38:16</v>
+      </c>
+      <c r="I17" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J17">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>20711</v>
+      </c>
+      <c r="B18" t="str">
+        <v>COSSIO DE DIAZ ROSSY FANNY</v>
+      </c>
+      <c r="C18">
+        <v>72206061</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+      <c r="E18" t="str">
+        <v>20</v>
+      </c>
+      <c r="F18" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G18" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H18" t="str">
+        <v>9:38:18</v>
+      </c>
+      <c r="I18" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J18">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>21502</v>
+      </c>
+      <c r="B19" t="str">
+        <v>COSSIO REY FABRICIO CRISTOBAL</v>
+      </c>
+      <c r="C19">
+        <v>76796433</v>
+      </c>
+      <c r="D19">
+        <v>30</v>
+      </c>
+      <c r="E19" t="str">
+        <v>20</v>
+      </c>
+      <c r="F19" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G19" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H19" t="str">
+        <v>9:38:20</v>
+      </c>
+      <c r="I19" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J19">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>39001</v>
+      </c>
+      <c r="B20" t="str">
+        <v>TORRICO SILES DE TEJERINA NANCY ROSARIO</v>
+      </c>
+      <c r="C20">
+        <v>70346980</v>
+      </c>
+      <c r="D20">
+        <v>30</v>
+      </c>
+      <c r="E20" t="str">
+        <v>20</v>
+      </c>
+      <c r="F20" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G20" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H20" t="str">
+        <v>9:38:22</v>
+      </c>
+      <c r="I20" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J20">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>2892</v>
+      </c>
+      <c r="B21" t="str">
+        <v>VARGAS ANGULO WILMER FRANCISCO</v>
+      </c>
+      <c r="C21">
+        <v>72777758</v>
+      </c>
+      <c r="D21">
+        <v>30</v>
+      </c>
+      <c r="E21" t="str">
+        <v>20</v>
+      </c>
+      <c r="F21" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G21" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H21" t="str">
+        <v>9:38:24</v>
+      </c>
+      <c r="I21" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J21">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>20711</v>
+      </c>
+      <c r="B22" t="str">
+        <v>COSSIO DE DIAZ ROSSY FANNY</v>
+      </c>
+      <c r="C22">
+        <v>72206061</v>
+      </c>
+      <c r="D22">
+        <v>30</v>
+      </c>
+      <c r="E22" t="str">
+        <v>20</v>
+      </c>
+      <c r="F22" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G22" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H22" t="str">
+        <v>9:38:26</v>
+      </c>
+      <c r="I22" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J22">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>21502</v>
+      </c>
+      <c r="B23" t="str">
+        <v>COSSIO REY FABRICIO CRISTOBAL</v>
+      </c>
+      <c r="C23">
+        <v>76796433</v>
+      </c>
+      <c r="D23">
+        <v>30</v>
+      </c>
+      <c r="E23" t="str">
+        <v>20</v>
+      </c>
+      <c r="F23" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G23" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H23" t="str">
+        <v>9:38:28</v>
+      </c>
+      <c r="I23" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J23">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>2892</v>
+      </c>
+      <c r="B24" t="str">
+        <v>VARGAS ANGULO WILMER FRANCISCO</v>
+      </c>
+      <c r="C24">
+        <v>72777758</v>
+      </c>
+      <c r="D24">
+        <v>30</v>
+      </c>
+      <c r="E24" t="str">
+        <v>20</v>
+      </c>
+      <c r="F24" t="str">
+        <v>VPR-ASFI Te invita a participar en la Encuesta Nacional de Servicios Financieros 2022 del 1/Dic al 31/Dic haz clic en: https://encuesta2022.asfi.gob.bo</v>
+      </c>
+      <c r="G24" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H24" t="str">
+        <v>10:20:6</v>
+      </c>
+      <c r="I24" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J24">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>20711</v>
+      </c>
+      <c r="B25" t="str">
+        <v>COSSIO DE DIAZ ROSSY FANNY</v>
+      </c>
+      <c r="C25">
+        <v>72206061</v>
+      </c>
+      <c r="D25">
+        <v>30</v>
+      </c>
+      <c r="E25" t="str">
+        <v>20</v>
+      </c>
+      <c r="F25" t="str">
+        <v>VPR-ASFI Te invita a participar en la Encuesta Nacional de Servicios Financieros 2022 del 1/Dic al 31/Dic haz clic en: https://encuesta2022.asfi.gob.bo</v>
+      </c>
+      <c r="G25" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H25" t="str">
+        <v>10:20:8</v>
+      </c>
+      <c r="I25" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J25">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>21502</v>
+      </c>
+      <c r="B26" t="str">
+        <v>COSSIO REY FABRICIO CRISTOBAL</v>
+      </c>
+      <c r="C26">
+        <v>76796433</v>
+      </c>
+      <c r="D26">
+        <v>30</v>
+      </c>
+      <c r="E26" t="str">
+        <v>20</v>
+      </c>
+      <c r="F26" t="str">
+        <v>VPR-ASFI Te invita a participar en la Encuesta Nacional de Servicios Financieros 2022 del 1/Dic al 31/Dic haz clic en: https://encuesta2022.asfi.gob.bo</v>
+      </c>
+      <c r="G26" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H26" t="str">
+        <v>10:20:10</v>
+      </c>
+      <c r="I26" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J26">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>39001</v>
+      </c>
+      <c r="B27" t="str">
+        <v>TORRICO SILES DE TEJERINA NANCY ROSARIO</v>
+      </c>
+      <c r="C27">
+        <v>70346980</v>
+      </c>
+      <c r="D27">
+        <v>30</v>
+      </c>
+      <c r="E27" t="str">
+        <v>20</v>
+      </c>
+      <c r="F27" t="str">
+        <v>VPR-ASFI Te invita a participar en la Encuesta Nacional de Servicios Financieros 2022 del 1/Dic al 31/Dic haz clic en: https://encuesta2022.asfi.gob.bo</v>
+      </c>
+      <c r="G27" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H27" t="str">
+        <v>10:20:12</v>
+      </c>
+      <c r="I27" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J27">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>2892</v>
+      </c>
+      <c r="B28" t="str">
+        <v>VARGAS ANGULO WILMER FRANCISCO</v>
+      </c>
+      <c r="C28">
+        <v>72777758</v>
+      </c>
+      <c r="D28">
+        <v>30</v>
+      </c>
+      <c r="E28" t="str">
+        <v>20</v>
+      </c>
+      <c r="F28" t="str">
+        <v>VPR-ASFI Te invita a participar en la Encuesta Nacional de Servicios Financieros 2022 del 1/Dic al 31/Dic haz clic en: https://encuesta2022.asfi.gob.bo</v>
+      </c>
+      <c r="G28" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H28" t="str">
+        <v>10:20:14</v>
+      </c>
+      <c r="I28" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J28">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>20711</v>
+      </c>
+      <c r="B29" t="str">
+        <v>COSSIO DE DIAZ ROSSY FANNY</v>
+      </c>
+      <c r="C29">
+        <v>72206061</v>
+      </c>
+      <c r="D29">
+        <v>30</v>
+      </c>
+      <c r="E29" t="str">
+        <v>20</v>
+      </c>
+      <c r="F29" t="str">
+        <v>VPR-ASFI Te invita a participar en la Encuesta Nacional de Servicios Financieros 2022 del 1/Dic al 31/Dic haz clic en: https://encuesta2022.asfi.gob.bo</v>
+      </c>
+      <c r="G29" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H29" t="str">
+        <v>10:20:16</v>
+      </c>
+      <c r="I29" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J29">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>21502</v>
+      </c>
+      <c r="B30" t="str">
+        <v>COSSIO REY FABRICIO CRISTOBAL</v>
+      </c>
+      <c r="C30">
+        <v>76796433</v>
+      </c>
+      <c r="D30">
+        <v>30</v>
+      </c>
+      <c r="E30" t="str">
+        <v>20</v>
+      </c>
+      <c r="F30" t="str">
+        <v>VPR-ASFI Te invita a participar en la Encuesta Nacional de Servicios Financieros 2022 del 1/Dic al 31/Dic haz clic en: https://encuesta2022.asfi.gob.bo</v>
+      </c>
+      <c r="G30" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H30" t="str">
+        <v>10:20:18</v>
+      </c>
+      <c r="I30" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J30">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>39001</v>
+      </c>
+      <c r="B31" t="str">
+        <v>TORRICO SILES DE TEJERINA NANCY ROSARIO</v>
+      </c>
+      <c r="C31">
+        <v>70346980</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+      <c r="E31" t="str">
+        <v>20</v>
+      </c>
+      <c r="F31" t="str">
+        <v>VPR-ASFI Te invita a participar en la Encuesta Nacional de Servicios Financieros 2022 del 1/Dic al 31/Dic haz clic en: https://encuesta2022.asfi.gob.bo</v>
+      </c>
+      <c r="G31" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H31" t="str">
+        <v>10:20:20</v>
+      </c>
+      <c r="I31" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J31">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>2892</v>
+      </c>
+      <c r="B32" t="str">
+        <v>VARGAS ANGULO WILMER FRANCISCO</v>
+      </c>
+      <c r="C32">
+        <v>72777758</v>
+      </c>
+      <c r="D32">
+        <v>30</v>
+      </c>
+      <c r="E32" t="str">
+        <v>20</v>
+      </c>
+      <c r="F32" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G32" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H32" t="str">
+        <v>10:42:49</v>
+      </c>
+      <c r="I32" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J32">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>20711</v>
+      </c>
+      <c r="B33" t="str">
+        <v>COSSIO DE DIAZ ROSSY FANNY</v>
+      </c>
+      <c r="C33">
+        <v>72206061</v>
+      </c>
+      <c r="D33">
+        <v>30</v>
+      </c>
+      <c r="E33" t="str">
+        <v>20</v>
+      </c>
+      <c r="F33" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G33" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H33" t="str">
+        <v>10:42:51</v>
+      </c>
+      <c r="I33" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J33">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>21502</v>
+      </c>
+      <c r="B34" t="str">
+        <v>COSSIO REY FABRICIO CRISTOBAL</v>
+      </c>
+      <c r="C34">
+        <v>76796433</v>
+      </c>
+      <c r="D34">
+        <v>30</v>
+      </c>
+      <c r="E34" t="str">
+        <v>20</v>
+      </c>
+      <c r="F34" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G34" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H34" t="str">
+        <v>10:42:53</v>
+      </c>
+      <c r="I34" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J34">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>39001</v>
+      </c>
+      <c r="B35" t="str">
+        <v>TORRICO SILES DE TEJERINA NANCY ROSARIO</v>
+      </c>
+      <c r="C35">
+        <v>70346980</v>
+      </c>
+      <c r="D35">
+        <v>30</v>
+      </c>
+      <c r="E35" t="str">
+        <v>20</v>
+      </c>
+      <c r="F35" t="str">
+        <v>este es un mensaje de prueba</v>
+      </c>
+      <c r="G35" t="str">
+        <v>20/1/2023</v>
+      </c>
+      <c r="H35" t="str">
+        <v>10:42:55</v>
+      </c>
+      <c r="I35" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J35">
+        <v>77487798</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>357643</v>
+      </c>
+      <c r="B36" t="str">
+        <v>CARDENAS SEJAS DIEGO PATRICK</v>
+      </c>
+      <c r="C36">
+        <v>79351361</v>
+      </c>
+      <c r="D36">
+        <v>30</v>
+      </c>
+      <c r="E36" t="str">
+        <v>30</v>
+      </c>
+      <c r="F36" t="str">
+        <v>VPR-ASFI Te invita a participar en la Encuesta Nacional de Servicios Financieros 2022 del 1/Dic al 31/Dic haz clic en: https://encuesta2022.asfi.gob.bo</v>
+      </c>
+      <c r="G36" t="str">
+        <v>21/1/2023</v>
+      </c>
+      <c r="H36" t="str">
+        <v>11:13:44</v>
+      </c>
+      <c r="I36" t="str">
+        <v>jose.crisolito@gmail.com</v>
+      </c>
+      <c r="J36">
+        <v>77487798</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J36"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>